<commit_message>
template integration of tob
</commit_message>
<xml_diff>
--- a/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/FCL_Backtrace_Start_simple_tob_en.xlsx
+++ b/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/FCL_Backtrace_Start_simple_tob_en.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>EAN</t>
   </si>
@@ -126,12 +126,15 @@
   <si>
     <t>[Country]</t>
   </si>
+  <si>
+    <t>[Business Type]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -391,6 +394,17 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1381,14 +1395,6 @@
     <xf numFmtId="49" fontId="35" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="35" fillId="4" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="36" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1401,18 +1407,61 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="36" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="36" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="36" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="36" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1479,51 +1528,15 @@
     <xf numFmtId="1" fontId="7" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="38" fillId="4" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1957,9 +1970,9 @@
     <col min="6" max="6" width="12.3984375" style="7" customWidth="1"/>
     <col min="7" max="7" width="12" style="7" customWidth="1"/>
     <col min="8" max="8" width="11.86328125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="4.3984375" style="30" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.73046875" style="30" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.265625" style="30" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.3984375" style="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.73046875" style="28" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.265625" style="28" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.265625" style="7" customWidth="1"/>
     <col min="13" max="13" width="32.3984375" style="7" customWidth="1"/>
     <col min="14" max="19" width="11.3984375" style="6"/>
@@ -1970,26 +1983,28 @@
       <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="27" t="s">
+      <c r="D1" s="64"/>
+      <c r="E1" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="F1" s="66" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="36"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="46"/>
       <c r="N1" s="23"/>
       <c r="O1" s="23"/>
       <c r="P1" s="23"/>
@@ -2007,187 +2022,187 @@
       <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="59"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
       <c r="M2" s="6"/>
     </row>
     <row r="3" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
       <c r="M3" s="6"/>
     </row>
     <row r="4" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="62"/>
-      <c r="L4" s="62"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
       <c r="M4" s="6"/>
     </row>
-    <row r="5" spans="1:19" s="29" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="65" t="s">
+    <row r="5" spans="1:19" s="27" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="28"/>
-    </row>
-    <row r="6" spans="1:19" s="29" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="63" t="s">
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+    </row>
+    <row r="6" spans="1:19" s="27" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="64"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="64"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="28"/>
-      <c r="S6" s="28"/>
-    </row>
-    <row r="7" spans="1:19" s="29" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="37" t="s">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+    </row>
+    <row r="7" spans="1:19" s="27" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="28"/>
-      <c r="Q7" s="28"/>
-      <c r="R7" s="28"/>
-      <c r="S7" s="28"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="26"/>
+      <c r="S7" s="26"/>
     </row>
     <row r="8" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="46" t="s">
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="47"/>
-      <c r="G8" s="46" t="s">
+      <c r="F8" s="57"/>
+      <c r="G8" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="47"/>
-      <c r="I8" s="51" t="s">
+      <c r="H8" s="57"/>
+      <c r="I8" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="39" t="s">
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="49" t="s">
         <v>10</v>
       </c>
       <c r="N8" s="13"/>
     </row>
     <row r="9" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C9" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="54" t="s">
+      <c r="E9" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="54" t="s">
+      <c r="F9" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="G9" s="54" t="s">
+      <c r="G9" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="54" t="s">
+      <c r="H9" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="56" t="s">
+      <c r="I9" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="57"/>
-      <c r="K9" s="58"/>
-      <c r="L9" s="54" t="s">
+      <c r="J9" s="31"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="M9" s="40"/>
+      <c r="M9" s="50"/>
       <c r="N9" s="13"/>
     </row>
     <row r="10" spans="1:19" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="43"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
+      <c r="A10" s="53"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
       <c r="I10" s="3" t="s">
         <v>11</v>
       </c>
@@ -2197,8 +2212,8 @@
       <c r="K10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L10" s="55"/>
-      <c r="M10" s="41"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="51"/>
       <c r="N10" s="13"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
@@ -2779,14 +2794,7 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="D2:L2"/>
-    <mergeCell ref="D3:L3"/>
-    <mergeCell ref="D4:L4"/>
-    <mergeCell ref="A6:M6"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C1:D1"/>
     <mergeCell ref="G1:M1"/>
     <mergeCell ref="A7:M7"/>
     <mergeCell ref="M8:M10"/>
@@ -2802,6 +2810,13 @@
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="D2:L2"/>
+    <mergeCell ref="D3:L3"/>
+    <mergeCell ref="D4:L4"/>
+    <mergeCell ref="A6:M6"/>
+    <mergeCell ref="A5:M5"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I11:I1048576">

</xml_diff>